<commit_message>
Final submission for the project.
</commit_message>
<xml_diff>
--- a/finalproject-gg-387-123.xlsx
+++ b/finalproject-gg-387-123.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="96">
   <si>
     <t>Students</t>
   </si>
@@ -262,9 +262,6 @@
     <t>3 bumpers</t>
   </si>
   <si>
-    <t>2 triangular slingshots</t>
-  </si>
-  <si>
     <t>1 plunger</t>
   </si>
   <si>
@@ -302,6 +299,15 @@
   </si>
   <si>
     <t>Used GJK algorithm to check collisions</t>
+  </si>
+  <si>
+    <t>With mediocre collisions it can only be so fun.</t>
+  </si>
+  <si>
+    <t>We have enough of a problem with failed response code that it feels like tunneling.</t>
+  </si>
+  <si>
+    <t>same as the section above</t>
   </si>
 </sst>
 </file>
@@ -652,6 +658,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -670,6 +685,39 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -700,24 +748,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -744,30 +774,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1087,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,58 +1109,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="53" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
       <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="50" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="55">
+      <c r="F2" s="59"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="40">
         <f>F78</f>
         <v>170</v>
       </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="47" t="s">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="48"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="41"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="12" t="s">
         <v>5</v>
       </c>
@@ -1170,25 +1176,25 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="3">
         <v>5</v>
       </c>
@@ -1202,12 +1208,12 @@
       <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="4">
         <v>5</v>
       </c>
@@ -1220,30 +1226,28 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
+      <c r="A8" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="4">
         <v>5</v>
       </c>
       <c r="F8" s="4">
-        <v>5</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>80</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G8" s="9"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="45"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
       <c r="E9" s="4">
         <v>5</v>
       </c>
@@ -1254,12 +1258,12 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:11" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
       <c r="E10" s="4">
         <v>5</v>
       </c>
@@ -1267,17 +1271,17 @@
         <v>5</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="58"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="14">
         <v>5</v>
       </c>
@@ -1288,25 +1292,25 @@
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="29"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="32"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="3">
         <v>10</v>
       </c>
@@ -1317,41 +1321,43 @@
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="29"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="32"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
+    <row r="15" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
       <c r="E15" s="3">
         <v>10</v>
       </c>
       <c r="F15" s="3">
-        <v>10</v>
-      </c>
-      <c r="G15" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
       <c r="E16" s="4">
         <v>10</v>
       </c>
@@ -1362,25 +1368,25 @@
       <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="29"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
       <c r="E18" s="3">
         <v>5</v>
       </c>
@@ -1391,25 +1397,25 @@
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="32"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
       <c r="E20" s="3">
         <v>5</v>
       </c>
@@ -1420,12 +1426,12 @@
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:9" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="45"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
       <c r="E21" s="14">
         <v>10</v>
       </c>
@@ -1433,30 +1439,30 @@
         <v>10</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="29"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="32"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="36"/>
       <c r="E23" s="3">
         <v>10</v>
       </c>
@@ -1467,12 +1473,12 @@
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:9" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="45"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26"/>
       <c r="E24" s="14">
         <v>10</v>
       </c>
@@ -1483,25 +1489,25 @@
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="29"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="32"/>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="36"/>
       <c r="E26" s="3">
         <v>10</v>
       </c>
@@ -1512,12 +1518,12 @@
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="45"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="26"/>
       <c r="E27" s="4">
         <v>10</v>
       </c>
@@ -1528,12 +1534,12 @@
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="4">
         <v>10</v>
       </c>
@@ -1541,46 +1547,48 @@
         <v>10</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="29"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="32"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
+    <row r="30" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="42"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="36"/>
       <c r="E30" s="3">
         <v>20</v>
       </c>
       <c r="F30" s="3">
-        <v>0</v>
-      </c>
-      <c r="G30" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="45"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="26"/>
       <c r="E31" s="4">
         <v>20</v>
       </c>
@@ -1591,12 +1599,12 @@
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="45"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
       <c r="E32" s="4">
         <v>20</v>
       </c>
@@ -1607,25 +1615,25 @@
       <c r="H32" s="15"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="29"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="32"/>
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="42"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="36"/>
       <c r="E34" s="3">
         <v>10</v>
       </c>
@@ -1633,17 +1641,17 @@
         <v>10</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="1:9" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="26"/>
       <c r="E35" s="4">
         <v>5</v>
       </c>
@@ -1651,17 +1659,17 @@
         <v>5</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H35" s="8"/>
     </row>
     <row r="36" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="45"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="26"/>
       <c r="E36" s="4">
         <v>5</v>
       </c>
@@ -1672,41 +1680,43 @@
       <c r="H36" s="15"/>
     </row>
     <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="29"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="32"/>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="42"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="36"/>
       <c r="E38" s="3">
         <v>10</v>
       </c>
       <c r="F38" s="3">
         <v>10</v>
       </c>
-      <c r="G38" s="6"/>
+      <c r="G38" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="H38" s="6"/>
     </row>
     <row r="39" spans="1:9" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="45"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="26"/>
       <c r="E39" s="4">
         <v>10</v>
       </c>
@@ -1717,12 +1727,12 @@
       <c r="H39" s="8"/>
     </row>
     <row r="40" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="43" t="s">
+      <c r="A40" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="44"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="45"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="26"/>
       <c r="E40" s="4">
         <v>10</v>
       </c>
@@ -1733,292 +1743,292 @@
       <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="29"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="32"/>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="42"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="36"/>
       <c r="E42" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
     </row>
     <row r="43" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="44"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="45"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="26"/>
       <c r="E43" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="16"/>
       <c r="H43" s="8"/>
     </row>
     <row r="44" spans="1:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="45"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="26"/>
       <c r="E44" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="9"/>
       <c r="H44" s="16"/>
     </row>
     <row r="45" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="45"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="26"/>
       <c r="E45" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="16"/>
       <c r="H45" s="8"/>
     </row>
     <row r="46" spans="1:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="44"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="45"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="26"/>
       <c r="E46" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="9"/>
       <c r="H46" s="16"/>
     </row>
     <row r="47" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="44"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="45"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="26"/>
       <c r="E47" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="16"/>
       <c r="H47" s="8"/>
     </row>
     <row r="48" spans="1:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="43" t="s">
+      <c r="A48" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="44"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="45"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="26"/>
       <c r="E48" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="9"/>
       <c r="H48" s="16"/>
     </row>
     <row r="49" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="43" t="s">
+      <c r="A49" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="45"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="26"/>
       <c r="E49" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="16"/>
       <c r="H49" s="8"/>
     </row>
     <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="43" t="s">
+      <c r="A50" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="44"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="45"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="26"/>
       <c r="E50" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="16"/>
       <c r="H50" s="8"/>
     </row>
     <row r="51" spans="1:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="59" t="s">
+      <c r="A51" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="60"/>
-      <c r="C51" s="60"/>
-      <c r="D51" s="61"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="39"/>
       <c r="E51" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="9"/>
       <c r="H51" s="16"/>
     </row>
     <row r="52" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="59" t="s">
+      <c r="A52" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="60"/>
-      <c r="C52" s="60"/>
-      <c r="D52" s="61"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="39"/>
       <c r="E52" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="16"/>
       <c r="H52" s="8"/>
     </row>
     <row r="53" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="59" t="s">
+      <c r="A53" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="60"/>
-      <c r="C53" s="60"/>
-      <c r="D53" s="61"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="39"/>
       <c r="E53" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H53" s="8"/>
     </row>
     <row r="54" spans="1:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="59" t="s">
+      <c r="A54" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="60"/>
-      <c r="C54" s="60"/>
-      <c r="D54" s="61"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="39"/>
       <c r="E54" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="9"/>
       <c r="H54" s="16"/>
     </row>
     <row r="55" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="59" t="s">
+      <c r="A55" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="60"/>
-      <c r="C55" s="60"/>
-      <c r="D55" s="61"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="39"/>
       <c r="E55" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="16"/>
       <c r="H55" s="8"/>
     </row>
     <row r="56" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="59" t="s">
+      <c r="A56" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="60"/>
-      <c r="C56" s="60"/>
-      <c r="D56" s="61"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="39"/>
       <c r="E56" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="16"/>
       <c r="H56" s="8"/>
     </row>
     <row r="57" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="59" t="s">
+      <c r="A57" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="60"/>
-      <c r="C57" s="60"/>
-      <c r="D57" s="61"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="39"/>
       <c r="E57" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="9"/>
       <c r="H57" s="16"/>
     </row>
     <row r="58" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="59" t="s">
+      <c r="A58" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="60"/>
-      <c r="C58" s="60"/>
-      <c r="D58" s="61"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="39"/>
       <c r="E58" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="16"/>
       <c r="H58" s="8"/>
     </row>
     <row r="59" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="59" t="s">
+      <c r="A59" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="60"/>
-      <c r="C59" s="60"/>
-      <c r="D59" s="61"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="39"/>
       <c r="E59" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="16"/>
       <c r="H59" s="8"/>
     </row>
     <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
+      <c r="A60" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="28"/>
-      <c r="H60" s="29"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="31"/>
+      <c r="H60" s="32"/>
       <c r="I60" s="1"/>
     </row>
     <row r="61" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="40" t="s">
+      <c r="A61" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="41"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="42"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="36"/>
       <c r="E61" s="3">
         <v>5</v>
       </c>
@@ -2029,12 +2039,12 @@
       <c r="H61" s="6"/>
     </row>
     <row r="62" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="43" t="s">
+      <c r="A62" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="44"/>
-      <c r="C62" s="44"/>
-      <c r="D62" s="45"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="26"/>
       <c r="E62" s="4">
         <v>5</v>
       </c>
@@ -2045,12 +2055,12 @@
       <c r="H62" s="8"/>
     </row>
     <row r="63" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="43" t="s">
+      <c r="A63" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="44"/>
-      <c r="C63" s="44"/>
-      <c r="D63" s="45"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="26"/>
       <c r="E63" s="4">
         <v>10</v>
       </c>
@@ -2061,12 +2071,12 @@
       <c r="H63" s="16"/>
     </row>
     <row r="64" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="43" t="s">
+      <c r="A64" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="44"/>
-      <c r="C64" s="44"/>
-      <c r="D64" s="45"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="26"/>
       <c r="E64" s="4">
         <v>10</v>
       </c>
@@ -2077,12 +2087,12 @@
       <c r="H64" s="8"/>
     </row>
     <row r="65" spans="1:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="43" t="s">
+      <c r="A65" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="44"/>
-      <c r="C65" s="44"/>
-      <c r="D65" s="45"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="26"/>
       <c r="E65" s="4">
         <v>10</v>
       </c>
@@ -2093,12 +2103,12 @@
       <c r="H65" s="16"/>
     </row>
     <row r="66" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="43" t="s">
+      <c r="A66" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="44"/>
-      <c r="C66" s="44"/>
-      <c r="D66" s="45"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="26"/>
       <c r="E66" s="4">
         <v>5</v>
       </c>
@@ -2109,12 +2119,12 @@
       <c r="H66" s="8"/>
     </row>
     <row r="67" spans="1:9" ht="74.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="43" t="s">
+      <c r="A67" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="44"/>
-      <c r="C67" s="44"/>
-      <c r="D67" s="45"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="26"/>
       <c r="E67" s="4">
         <v>10</v>
       </c>
@@ -2125,12 +2135,12 @@
       <c r="H67" s="16"/>
     </row>
     <row r="68" spans="1:9" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="43" t="s">
+      <c r="A68" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="44"/>
-      <c r="C68" s="44"/>
-      <c r="D68" s="45"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="26"/>
       <c r="E68" s="4">
         <v>20</v>
       </c>
@@ -2141,12 +2151,12 @@
       <c r="H68" s="8"/>
     </row>
     <row r="69" spans="1:9" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="43" t="s">
+      <c r="A69" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="44"/>
-      <c r="C69" s="44"/>
-      <c r="D69" s="45"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="26"/>
       <c r="E69" s="4">
         <v>10</v>
       </c>
@@ -2157,12 +2167,12 @@
       <c r="H69" s="16"/>
     </row>
     <row r="70" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="43" t="s">
+      <c r="A70" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="44"/>
-      <c r="C70" s="44"/>
-      <c r="D70" s="45"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="26"/>
       <c r="E70" s="4">
         <v>10</v>
       </c>
@@ -2173,12 +2183,12 @@
       <c r="H70" s="8"/>
     </row>
     <row r="71" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="43" t="s">
+      <c r="A71" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="44"/>
-      <c r="C71" s="44"/>
-      <c r="D71" s="45"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="26"/>
       <c r="E71" s="4">
         <v>30</v>
       </c>
@@ -2189,12 +2199,12 @@
       <c r="H71" s="16"/>
     </row>
     <row r="72" spans="1:9" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="43" t="s">
+      <c r="A72" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="44"/>
-      <c r="C72" s="44"/>
-      <c r="D72" s="45"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="26"/>
       <c r="E72" s="4">
         <v>40</v>
       </c>
@@ -2205,12 +2215,12 @@
       <c r="H72" s="8"/>
     </row>
     <row r="73" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="43" t="s">
+      <c r="A73" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="44"/>
-      <c r="C73" s="44"/>
-      <c r="D73" s="45"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
+      <c r="D73" s="26"/>
       <c r="E73" s="4">
         <v>100</v>
       </c>
@@ -2221,12 +2231,12 @@
       <c r="H73" s="8"/>
     </row>
     <row r="74" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="B74" s="38"/>
-      <c r="C74" s="38"/>
-      <c r="D74" s="39"/>
+      <c r="A74" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="B74" s="52"/>
+      <c r="C74" s="52"/>
+      <c r="D74" s="53"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4">
         <v>20</v>
@@ -2235,28 +2245,28 @@
       <c r="H74" s="8"/>
     </row>
     <row r="75" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="B75" s="38"/>
-      <c r="C75" s="38"/>
-      <c r="D75" s="39"/>
+      <c r="A75" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="B75" s="52"/>
+      <c r="C75" s="52"/>
+      <c r="D75" s="53"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4">
         <v>20</v>
       </c>
       <c r="G75" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H75" s="8"/>
+    </row>
+    <row r="76" spans="1:9" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="H75" s="8"/>
-    </row>
-    <row r="76" spans="1:9" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="B76" s="44"/>
-      <c r="C76" s="44"/>
-      <c r="D76" s="45"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="26"/>
       <c r="E76" s="4" t="s">
         <v>74</v>
       </c>
@@ -2264,28 +2274,28 @@
         <v>10</v>
       </c>
       <c r="G76" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H76" s="8"/>
     </row>
     <row r="77" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="24" t="s">
+      <c r="A77" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="26"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="28"/>
-      <c r="G77" s="28"/>
-      <c r="H77" s="29"/>
+      <c r="B77" s="28"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="30"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
+      <c r="H77" s="32"/>
       <c r="I77" s="1"/>
     </row>
     <row r="78" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="62"/>
-      <c r="B78" s="62"/>
-      <c r="C78" s="62"/>
-      <c r="D78" s="62"/>
+      <c r="A78" s="33"/>
+      <c r="B78" s="33"/>
+      <c r="C78" s="33"/>
+      <c r="D78" s="33"/>
       <c r="E78" s="21">
         <f>SUM(E4:E40)</f>
         <v>240</v>
@@ -2525,46 +2535,43 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="E77:H77"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="E60:H60"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="E41:H41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E22:H22"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="A13:D13"/>
@@ -2581,43 +2588,46 @@
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="A31:D31"/>
     <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="E33:H33"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="E41:H41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="E60:H60"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="E77:H77"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="A73:D73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>